<commit_message>
Acrescentei o método groupby para filtrar as colunas e os valores que quero no relatório
</commit_message>
<xml_diff>
--- a/vendas.xlsx
+++ b/vendas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Área de Trabalho\Relatorio de Vendas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E285D68A-3A25-43A8-A3C7-AC757EFEC02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBFB4E6-5FC0-4F3D-BCFF-CF7598A4C97D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{9BFD011F-1C39-46B9-BCAD-7D80E13B3DBC}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="18000" windowHeight="9360" xr2:uid="{9BFD011F-1C39-46B9-BCAD-7D80E13B3DBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -41,85 +41,85 @@
     <t>Data</t>
   </si>
   <si>
+    <t>Produto</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
+  <si>
+    <t>Valor unitário</t>
+  </si>
+  <si>
+    <t>Valor final</t>
+  </si>
+  <si>
+    <t>Loja 1</t>
+  </si>
+  <si>
+    <t>Loja 2</t>
+  </si>
+  <si>
+    <t>Loja 3</t>
+  </si>
+  <si>
+    <t>Loja 4</t>
+  </si>
+  <si>
+    <t>Loja 5</t>
+  </si>
+  <si>
+    <t>Loja 6</t>
+  </si>
+  <si>
+    <t>Loja 7</t>
+  </si>
+  <si>
+    <t>Loja 8</t>
+  </si>
+  <si>
+    <t>Loja 9</t>
+  </si>
+  <si>
+    <t>Loja 10</t>
+  </si>
+  <si>
+    <t>Sapato</t>
+  </si>
+  <si>
+    <t>Camisa</t>
+  </si>
+  <si>
+    <t>Sapato Xadrez</t>
+  </si>
+  <si>
+    <t>Bolsa</t>
+  </si>
+  <si>
+    <t>Camiseta</t>
+  </si>
+  <si>
+    <t>Tênis</t>
+  </si>
+  <si>
+    <t>Calça</t>
+  </si>
+  <si>
+    <t>Camisa Polo</t>
+  </si>
+  <si>
+    <t>Casaco</t>
+  </si>
+  <si>
+    <t>Sandália</t>
+  </si>
+  <si>
+    <t>Biquini</t>
+  </si>
+  <si>
+    <t>Sunga</t>
+  </si>
+  <si>
     <t>ID Loja</t>
-  </si>
-  <si>
-    <t>Produto</t>
-  </si>
-  <si>
-    <t>Quantidade</t>
-  </si>
-  <si>
-    <t>Valor unitário</t>
-  </si>
-  <si>
-    <t>Valor final</t>
-  </si>
-  <si>
-    <t>Loja 1</t>
-  </si>
-  <si>
-    <t>Loja 2</t>
-  </si>
-  <si>
-    <t>Loja 3</t>
-  </si>
-  <si>
-    <t>Loja 4</t>
-  </si>
-  <si>
-    <t>Loja 5</t>
-  </si>
-  <si>
-    <t>Loja 6</t>
-  </si>
-  <si>
-    <t>Loja 7</t>
-  </si>
-  <si>
-    <t>Loja 8</t>
-  </si>
-  <si>
-    <t>Loja 9</t>
-  </si>
-  <si>
-    <t>Loja 10</t>
-  </si>
-  <si>
-    <t>Sapato</t>
-  </si>
-  <si>
-    <t>Camisa</t>
-  </si>
-  <si>
-    <t>Sapato Xadrez</t>
-  </si>
-  <si>
-    <t>Bolsa</t>
-  </si>
-  <si>
-    <t>Camiseta</t>
-  </si>
-  <si>
-    <t>Tênis</t>
-  </si>
-  <si>
-    <t>Calça</t>
-  </si>
-  <si>
-    <t>Camisa Polo</t>
-  </si>
-  <si>
-    <t>Casaco</t>
-  </si>
-  <si>
-    <t>Sandália</t>
-  </si>
-  <si>
-    <t>Biquini</t>
-  </si>
-  <si>
-    <t>Sunga</t>
   </si>
 </sst>
 </file>
@@ -128,7 +128,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -162,7 +162,7 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -483,7 +483,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,19 +504,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -527,10 +527,10 @@
         <v>44562</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -550,10 +550,10 @@
         <v>44562</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -573,10 +573,10 @@
         <v>44562</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -596,10 +596,10 @@
         <v>44563</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -619,10 +619,10 @@
         <v>44593</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -642,10 +642,10 @@
         <v>44594</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -665,10 +665,10 @@
         <v>44621</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -688,10 +688,10 @@
         <v>44652</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -711,10 +711,10 @@
         <v>44682</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -734,10 +734,10 @@
         <v>44713</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -757,10 +757,10 @@
         <v>44713</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -780,10 +780,10 @@
         <v>44714</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -803,10 +803,10 @@
         <v>44714</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -826,10 +826,10 @@
         <v>44714</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -849,10 +849,10 @@
         <v>44743</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -872,10 +872,10 @@
         <v>44743</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E17">
         <v>1</v>

</xml_diff>